<commit_message>
fixed chart formatting, cleaned up data formatting in excel charts
</commit_message>
<xml_diff>
--- a/excel_data/11 - November/2020-11-14.xlsx
+++ b/excel_data/11 - November/2020-11-14.xlsx
@@ -15,261 +15,261 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="87">
+  <si>
+    <t>Bear Position</t>
+  </si>
+  <si>
+    <t>Bull Position</t>
+  </si>
+  <si>
+    <t>Ticker</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>ACB</t>
+  </si>
+  <si>
+    <t>AMD</t>
+  </si>
+  <si>
+    <t>AMZN</t>
+  </si>
+  <si>
+    <t>APHA</t>
+  </si>
+  <si>
+    <t>ARK</t>
+  </si>
+  <si>
+    <t>ATM</t>
+  </si>
+  <si>
+    <t>ATVI</t>
+  </si>
+  <si>
+    <t>BA</t>
+  </si>
+  <si>
+    <t>BABA</t>
+  </si>
+  <si>
+    <t>BBY</t>
+  </si>
+  <si>
+    <t>BJ</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>CCL</t>
+  </si>
+  <si>
+    <t>COST</t>
+  </si>
+  <si>
+    <t>CSIQ</t>
+  </si>
+  <si>
+    <t>DEFINITELY</t>
+  </si>
+  <si>
+    <t>DG</t>
+  </si>
+  <si>
+    <t>DIA</t>
+  </si>
+  <si>
+    <t>DTE</t>
+  </si>
+  <si>
+    <t>ER</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>FB</t>
+  </si>
+  <si>
+    <t>FD</t>
+  </si>
+  <si>
+    <t>FSLY</t>
+  </si>
+  <si>
+    <t>FSR</t>
+  </si>
+  <si>
+    <t>GILD</t>
+  </si>
+  <si>
+    <t>GME</t>
+  </si>
+  <si>
+    <t>HYG</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>IBUY</t>
+  </si>
+  <si>
+    <t>ICLN</t>
+  </si>
+  <si>
+    <t>ITM</t>
+  </si>
+  <si>
+    <t>IV</t>
+  </si>
+  <si>
+    <t>IWM</t>
+  </si>
+  <si>
+    <t>JD</t>
+  </si>
+  <si>
+    <t>JMIA</t>
+  </si>
+  <si>
+    <t>KR</t>
+  </si>
+  <si>
+    <t>LI</t>
+  </si>
+  <si>
+    <t>LK</t>
+  </si>
+  <si>
+    <t>LYFT</t>
+  </si>
+  <si>
+    <t>MRNA</t>
+  </si>
+  <si>
+    <t>MRVL</t>
+  </si>
+  <si>
+    <t>MSFT</t>
+  </si>
+  <si>
+    <t>NAK</t>
+  </si>
+  <si>
+    <t>NIO</t>
+  </si>
+  <si>
+    <t>NKLA</t>
+  </si>
+  <si>
+    <t>NLS</t>
+  </si>
+  <si>
+    <t>NVDA</t>
+  </si>
+  <si>
+    <t>NVTA</t>
+  </si>
+  <si>
+    <t>OTM</t>
+  </si>
+  <si>
+    <t>OWL</t>
+  </si>
+  <si>
+    <t>OXY</t>
+  </si>
+  <si>
+    <t>PFE</t>
+  </si>
+  <si>
+    <t>PINS</t>
+  </si>
+  <si>
+    <t>PLTR</t>
+  </si>
+  <si>
+    <t>PTON</t>
+  </si>
+  <si>
+    <t>QQQ</t>
+  </si>
+  <si>
+    <t>RCL</t>
+  </si>
+  <si>
+    <t>ROKU</t>
+  </si>
+  <si>
+    <t>ROPE</t>
+  </si>
+  <si>
+    <t>SE</t>
+  </si>
+  <si>
+    <t>SOLO</t>
+  </si>
+  <si>
+    <t>SPCE</t>
+  </si>
+  <si>
+    <t>SPXS</t>
+  </si>
+  <si>
+    <t>SPY</t>
+  </si>
+  <si>
+    <t>STO</t>
+  </si>
+  <si>
+    <t>TDOC</t>
+  </si>
+  <si>
+    <t>TGT</t>
+  </si>
+  <si>
+    <t>TQQQ</t>
+  </si>
+  <si>
+    <t>TSLA</t>
+  </si>
+  <si>
+    <t>UAL</t>
+  </si>
+  <si>
+    <t>UBER</t>
+  </si>
+  <si>
+    <t>UUP</t>
+  </si>
+  <si>
+    <t>UVXY</t>
+  </si>
+  <si>
+    <t>VIX</t>
+  </si>
+  <si>
+    <t>VXX</t>
+  </si>
+  <si>
+    <t>WMT</t>
+  </si>
+  <si>
+    <t>WORK</t>
+  </si>
+  <si>
+    <t>XOP</t>
+  </si>
+  <si>
+    <t>ZM</t>
+  </si>
   <si>
     <t>Position</t>
-  </si>
-  <si>
-    <t>Ticker</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>ACB</t>
-  </si>
-  <si>
-    <t>AMD</t>
-  </si>
-  <si>
-    <t>AMZN</t>
-  </si>
-  <si>
-    <t>APHA</t>
-  </si>
-  <si>
-    <t>ARK</t>
-  </si>
-  <si>
-    <t>BA</t>
-  </si>
-  <si>
-    <t>BABA</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>CCL</t>
-  </si>
-  <si>
-    <t>COST</t>
-  </si>
-  <si>
-    <t>CSIQ</t>
-  </si>
-  <si>
-    <t>DG</t>
-  </si>
-  <si>
-    <t>DTE</t>
-  </si>
-  <si>
-    <t>ER</t>
-  </si>
-  <si>
-    <t>FB</t>
-  </si>
-  <si>
-    <t>FD</t>
-  </si>
-  <si>
-    <t>FSR</t>
-  </si>
-  <si>
-    <t>GILD</t>
-  </si>
-  <si>
-    <t>GME</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t>IBUY</t>
-  </si>
-  <si>
-    <t>ICLN</t>
-  </si>
-  <si>
-    <t>ITM</t>
-  </si>
-  <si>
-    <t>IWM</t>
-  </si>
-  <si>
-    <t>JD</t>
-  </si>
-  <si>
-    <t>JMIA</t>
-  </si>
-  <si>
-    <t>KR</t>
-  </si>
-  <si>
-    <t>LI</t>
-  </si>
-  <si>
-    <t>LK</t>
-  </si>
-  <si>
-    <t>MRNA</t>
-  </si>
-  <si>
-    <t>MSFT</t>
-  </si>
-  <si>
-    <t>NAK</t>
-  </si>
-  <si>
-    <t>NIO</t>
-  </si>
-  <si>
-    <t>NLS</t>
-  </si>
-  <si>
-    <t>NVDA</t>
-  </si>
-  <si>
-    <t>NVTA</t>
-  </si>
-  <si>
-    <t>OTM</t>
-  </si>
-  <si>
-    <t>OWL</t>
-  </si>
-  <si>
-    <t>OXY</t>
-  </si>
-  <si>
-    <t>PFE</t>
-  </si>
-  <si>
-    <t>PINS</t>
-  </si>
-  <si>
-    <t>PLTR</t>
-  </si>
-  <si>
-    <t>PTON</t>
-  </si>
-  <si>
-    <t>QQQ</t>
-  </si>
-  <si>
-    <t>ROKU</t>
-  </si>
-  <si>
-    <t>ROPE</t>
-  </si>
-  <si>
-    <t>SE</t>
-  </si>
-  <si>
-    <t>SOLO</t>
-  </si>
-  <si>
-    <t>SPCE</t>
-  </si>
-  <si>
-    <t>SPY</t>
-  </si>
-  <si>
-    <t>TDOC</t>
-  </si>
-  <si>
-    <t>TGT</t>
-  </si>
-  <si>
-    <t>TQQQ</t>
-  </si>
-  <si>
-    <t>TSLA</t>
-  </si>
-  <si>
-    <t>UBER</t>
-  </si>
-  <si>
-    <t>UUP</t>
-  </si>
-  <si>
-    <t>UVXY</t>
-  </si>
-  <si>
-    <t>VIX</t>
-  </si>
-  <si>
-    <t>VXX</t>
-  </si>
-  <si>
-    <t>WMT</t>
-  </si>
-  <si>
-    <t>WORK</t>
-  </si>
-  <si>
-    <t>ZM</t>
-  </si>
-  <si>
-    <t>calls</t>
-  </si>
-  <si>
-    <t>ATM</t>
-  </si>
-  <si>
-    <t>ATVI</t>
-  </si>
-  <si>
-    <t>BBY</t>
-  </si>
-  <si>
-    <t>BJ</t>
-  </si>
-  <si>
-    <t>DEFINITELY</t>
-  </si>
-  <si>
-    <t>DIA</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>FSLY</t>
-  </si>
-  <si>
-    <t>HYG</t>
-  </si>
-  <si>
-    <t>IV</t>
-  </si>
-  <si>
-    <t>LYFT</t>
-  </si>
-  <si>
-    <t>MRVL</t>
-  </si>
-  <si>
-    <t>NKLA</t>
-  </si>
-  <si>
-    <t>RCL</t>
-  </si>
-  <si>
-    <t>SPXS</t>
-  </si>
-  <si>
-    <t>STO</t>
-  </si>
-  <si>
-    <t>UAL</t>
-  </si>
-  <si>
-    <t>XOP</t>
-  </si>
-  <si>
-    <t>puts</t>
   </si>
   <si>
     <t>FIT</t>
@@ -366,22 +366,22 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Position</c:v>
+                  <c:v>Bear Position</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$A$64</c:f>
+              <c:f>Sheet1!$B$2:$A$82</c:f>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$64</c:f>
+              <c:f>Sheet1!$C$2:$C$82</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="63"/>
+                <c:ptCount val="81"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -389,112 +389,112 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="27">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="30">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="31">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="23">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>1</c:v>
-                </c:pt>
                 <c:pt idx="32">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>48</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="34">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="35">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="36">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="36">
-                  <c:v>1</c:v>
-                </c:pt>
                 <c:pt idx="37">
-                  <c:v>16</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>1</c:v>
@@ -503,72 +503,126 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="41">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="43">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>4</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>1</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="47">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="49">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="50">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="65">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="51">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="66">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="68">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="53">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="69">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="70">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="55">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="57">
+                <c:pt idx="71">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="74">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="58">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="59">
+                <c:pt idx="75">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="76">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="60">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="62">
+                <c:pt idx="77">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="80">
                   <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
@@ -699,13 +753,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
@@ -1050,7 +1104,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C64"/>
+  <dimension ref="A1:C82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1058,21 +1112,21 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>84</v>
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1080,10 +1134,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>84</v>
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1091,43 +1145,43 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>84</v>
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>84</v>
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>84</v>
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>84</v>
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1135,32 +1189,32 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>84</v>
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>84</v>
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>84</v>
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1168,43 +1222,43 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>84</v>
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>84</v>
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>84</v>
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>84</v>
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -1212,10 +1266,10 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>84</v>
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -1223,21 +1277,21 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>84</v>
+        <v>17</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
       </c>
       <c r="C16">
-        <v>19</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>84</v>
+        <v>18</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -1245,21 +1299,21 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>84</v>
+        <v>19</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>84</v>
+        <v>20</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -1267,32 +1321,32 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>84</v>
+        <v>21</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>84</v>
+        <v>22</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>84</v>
+        <v>23</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -1300,54 +1354,54 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>84</v>
+        <v>24</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
       </c>
       <c r="C23">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>84</v>
+        <v>25</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
       </c>
       <c r="C24">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>84</v>
+        <v>26</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
       </c>
       <c r="C25">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>84</v>
+        <v>27</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
       </c>
       <c r="C26">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>84</v>
+        <v>28</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -1355,98 +1409,98 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>84</v>
+        <v>29</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
       </c>
       <c r="C28">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>84</v>
+        <v>30</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
       </c>
       <c r="C29">
-        <v>18</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>84</v>
+        <v>31</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
       </c>
       <c r="C30">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>84</v>
+        <v>32</v>
+      </c>
+      <c r="B31">
+        <v>19</v>
       </c>
       <c r="C31">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>84</v>
+        <v>33</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
       </c>
       <c r="C32">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>84</v>
+        <v>34</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
       </c>
       <c r="C33">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>84</v>
+        <v>35</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
       </c>
       <c r="C34">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>65</v>
+        <v>36</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
       </c>
       <c r="C35">
-        <v>48</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>65</v>
+        <v>37</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
       </c>
       <c r="C36">
         <v>2</v>
@@ -1454,43 +1508,43 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>65</v>
+        <v>38</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
       </c>
       <c r="C37">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>65</v>
+        <v>39</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
       </c>
       <c r="C38">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>65</v>
+        <v>40</v>
+      </c>
+      <c r="B39">
+        <v>0</v>
       </c>
       <c r="C39">
-        <v>16</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>65</v>
+        <v>41</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -1498,10 +1552,10 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>65</v>
+        <v>42</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
       </c>
       <c r="C41">
         <v>1</v>
@@ -1509,21 +1563,21 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>65</v>
+        <v>43</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
       </c>
       <c r="C42">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>65</v>
+        <v>44</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -1531,21 +1585,21 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>65</v>
+        <v>45</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
       </c>
       <c r="C44">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>65</v>
+        <v>46</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
       </c>
       <c r="C45">
         <v>2</v>
@@ -1553,43 +1607,43 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>65</v>
+        <v>47</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
       </c>
       <c r="C46">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>65</v>
+        <v>48</v>
+      </c>
+      <c r="B47">
+        <v>8</v>
       </c>
       <c r="C47">
-        <v>1</v>
+        <v>48</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>65</v>
+        <v>49</v>
+      </c>
+      <c r="B48">
+        <v>2</v>
       </c>
       <c r="C48">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>65</v>
+        <v>50</v>
+      </c>
+      <c r="B49">
+        <v>0</v>
       </c>
       <c r="C49">
         <v>2</v>
@@ -1597,21 +1651,21 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>65</v>
+        <v>51</v>
+      </c>
+      <c r="B50">
+        <v>0</v>
       </c>
       <c r="C50">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>65</v>
+        <v>52</v>
+      </c>
+      <c r="B51">
+        <v>0</v>
       </c>
       <c r="C51">
         <v>1</v>
@@ -1619,21 +1673,21 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>65</v>
+        <v>53</v>
+      </c>
+      <c r="B52">
+        <v>4</v>
       </c>
       <c r="C52">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>65</v>
+        <v>54</v>
+      </c>
+      <c r="B53">
+        <v>0</v>
       </c>
       <c r="C53">
         <v>1</v>
@@ -1641,98 +1695,98 @@
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>65</v>
+        <v>55</v>
+      </c>
+      <c r="B54">
+        <v>0</v>
       </c>
       <c r="C54">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>65</v>
+        <v>56</v>
+      </c>
+      <c r="B55">
+        <v>0</v>
       </c>
       <c r="C55">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>65</v>
+        <v>57</v>
+      </c>
+      <c r="B56">
+        <v>0</v>
       </c>
       <c r="C56">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>65</v>
+        <v>58</v>
+      </c>
+      <c r="B57">
+        <v>0</v>
       </c>
       <c r="C57">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
+      </c>
+      <c r="B58">
+        <v>0</v>
       </c>
       <c r="C58">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
+      </c>
+      <c r="B59">
+        <v>0</v>
       </c>
       <c r="C59">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
+      </c>
+      <c r="B60">
+        <v>1</v>
       </c>
       <c r="C60">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
+      </c>
+      <c r="B61">
+        <v>0</v>
       </c>
       <c r="C61">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
+      </c>
+      <c r="B62">
+        <v>0</v>
       </c>
       <c r="C62">
         <v>1</v>
@@ -1740,23 +1794,221 @@
     </row>
     <row r="63" spans="1:3">
       <c r="A63" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
+      </c>
+      <c r="B63">
+        <v>0</v>
       </c>
       <c r="C63">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B64" s="1" t="s">
         <v>65</v>
       </c>
+      <c r="B64">
+        <v>1</v>
+      </c>
       <c r="C64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B65">
+        <v>0</v>
+      </c>
+      <c r="C65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B66">
+        <v>2</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B67">
+        <v>18</v>
+      </c>
+      <c r="C67">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B68">
+        <v>1</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B69">
+        <v>0</v>
+      </c>
+      <c r="C69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B70">
+        <v>0</v>
+      </c>
+      <c r="C70">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B71">
+        <v>0</v>
+      </c>
+      <c r="C71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B72">
+        <v>0</v>
+      </c>
+      <c r="C72">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B73">
+        <v>1</v>
+      </c>
+      <c r="C73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B74">
+        <v>2</v>
+      </c>
+      <c r="C74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B75">
+        <v>0</v>
+      </c>
+      <c r="C75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B76">
+        <v>0</v>
+      </c>
+      <c r="C76">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B77">
+        <v>0</v>
+      </c>
+      <c r="C77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B78">
+        <v>0</v>
+      </c>
+      <c r="C78">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B79">
+        <v>0</v>
+      </c>
+      <c r="C79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B80">
+        <v>0</v>
+      </c>
+      <c r="C80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B81">
+        <v>1</v>
+      </c>
+      <c r="C81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B82">
+        <v>4</v>
+      </c>
+      <c r="C82">
         <v>8</v>
       </c>
     </row>
@@ -1776,10 +2028,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1792,7 +2044,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1800,7 +2052,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1808,7 +2060,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -1824,7 +2076,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="B7">
         <v>5</v>
@@ -1832,7 +2084,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -1840,7 +2092,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1848,7 +2100,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1856,7 +2108,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="B11">
         <v>1</v>

</xml_diff>